<commit_message>
Added Jacob and Ally onto the website
</commit_message>
<xml_diff>
--- a/src/data/summerfall23/bios_summerfall23.xlsx
+++ b/src/data/summerfall23/bios_summerfall23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\summerfall23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C05DF99-6F3E-4A20-9824-79321E176BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F4835A-FC64-41FE-A0B2-C30CF3CE627B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="3090" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2715" yWindow="450" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="513">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1438,9 +1438,6 @@
     <t>Marketing, UI/UX Design</t>
   </si>
   <si>
-    <t xml:space="preserve">Communications, Advocacy </t>
-  </si>
-  <si>
     <t>Social Media Marketing Manager @ Niche Street</t>
   </si>
   <si>
@@ -1508,6 +1505,60 @@
   </si>
   <si>
     <t>Marketing Program Management Intern @ Duolingo</t>
+  </si>
+  <si>
+    <t>jacob_lee</t>
+  </si>
+  <si>
+    <t>Communications, Advocacy</t>
+  </si>
+  <si>
+    <t>Consulting, Finance, Wealth Management</t>
+  </si>
+  <si>
+    <t>ASUCI, KCM</t>
+  </si>
+  <si>
+    <t>Hi! My name is Jacob Lee and I initiated the Spring quarter of my first year with the Alpha Omicron class. In my free time, I love driving around to get food with friends, watching Netflix, being outdoors, as well as playing volleyball and soccer. Feel free to ask me about my favorite shows, food, or anything else at recruitment!</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/jacobjlee2004/</t>
+  </si>
+  <si>
+    <t>jacoblee@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Allison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chu </t>
+  </si>
+  <si>
+    <t>allison_chu</t>
+  </si>
+  <si>
+    <t>Anaheim Hills, CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psychology </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI/UX design, Product Design, Product Management </t>
+  </si>
+  <si>
+    <t>Intern @ BCA Watson Rice LLP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpha Phi, MAISS, Kaba Modern </t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/allisonichu/</t>
+  </si>
+  <si>
+    <t>allisonchu@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hi hi! My name is Alli, and I initiated spring of my second year with the Alpha Omicron class. In my free time, I love to dance, snowboard, go to the beach, and travel. A fun fact is that I have a deadly phobia of snails! Feel free to ask me about my favorite TV shows to binge watch, and why elephants are the best animals in the world — I can't wait to meet everyone!</t>
   </si>
 </sst>
 </file>
@@ -1944,13 +1995,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2035,7 +2086,7 @@
         <v>379</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>460</v>
@@ -2045,7 +2096,7 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>472</v>
+        <v>496</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>461</v>
@@ -2442,484 +2493,487 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>505</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>507</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>508</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>509</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>510</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>511</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>44404.652777777781</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N11" s="7" t="s">
+      <c r="N12" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="O11" s="7" t="s">
+      <c r="O12" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="P12" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="15">
+    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="15">
         <v>44397.381944444445</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>117</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N12" s="7" t="s">
+      <c r="N13" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="O12" s="7" t="s">
+      <c r="O13" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
+    <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2" t="s">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N14" t="s">
         <v>279</v>
       </c>
-      <c r="O13" s="8" t="s">
+      <c r="O14" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="P14" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2" t="s">
+    <row r="15" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I15" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="N15" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="15">
+    <row r="16" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="15">
         <v>44397.802083333336</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>333</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N15" t="s">
-        <v>112</v>
-      </c>
-      <c r="O15" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="2"/>
+      <c r="I16" s="11" t="s">
+        <v>333</v>
+      </c>
       <c r="J16" s="2" t="s">
-        <v>142</v>
+        <v>356</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>21</v>
+        <v>357</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>21</v>
+        <v>358</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>143</v>
+        <v>39</v>
+      </c>
+      <c r="N16" t="s">
+        <v>112</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
-        <v>440</v>
+        <v>138</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>441</v>
+        <v>139</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>442</v>
+        <v>140</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>379</v>
+        <v>117</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>34</v>
+        <v>141</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>443</v>
+        <v>142</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>444</v>
+        <v>21</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="O17" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="P17" s="16" t="s">
-        <v>447</v>
+        <v>158</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
-        <v>123</v>
+        <v>440</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>124</v>
+        <v>441</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>125</v>
+        <v>442</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>117</v>
+        <v>379</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>126</v>
+        <v>34</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>320</v>
-      </c>
+      <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="L18" s="10" t="s">
-        <v>322</v>
+        <v>443</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>444</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N18" t="s">
-        <v>157</v>
+        <v>33</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>445</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>128</v>
+        <v>446</v>
+      </c>
+      <c r="P18" s="16" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>296</v>
+        <v>123</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>297</v>
+        <v>124</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E19" t="s">
-        <v>242</v>
+        <v>125</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>299</v>
+        <v>126</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>320</v>
+      </c>
       <c r="J19" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>302</v>
+        <v>321</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>322</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>305</v>
+        <v>35</v>
+      </c>
+      <c r="N19" t="s">
+        <v>157</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>304</v>
+        <v>127</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>303</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>477</v>
+        <v>296</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>478</v>
+        <v>297</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>379</v>
+        <v>298</v>
+      </c>
+      <c r="E20" t="s">
+        <v>242</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>388</v>
+        <v>299</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="K20" s="16" t="s">
-        <v>481</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>482</v>
+        <v>300</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>302</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>483</v>
+        <v>305</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>484</v>
+        <v>304</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>404</v>
+        <v>476</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>115</v>
+        <v>477</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>405</v>
+        <v>478</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>379</v>
@@ -2928,43 +2982,42 @@
         <v>27</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="16" t="s">
-        <v>407</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M21" s="11" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>480</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>481</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>408</v>
+        <v>482</v>
       </c>
       <c r="O21" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="P21" s="16" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+        <v>483</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>468</v>
+        <v>404</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>115</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>469</v>
+        <v>405</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>379</v>
@@ -2973,419 +3026,413 @@
         <v>27</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>15</v>
+        <v>406</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>470</v>
-      </c>
+      <c r="I22" s="2"/>
       <c r="J22" s="16" t="s">
-        <v>471</v>
-      </c>
-      <c r="K22" s="16" t="s">
-        <v>473</v>
-      </c>
-      <c r="L22" s="16" t="s">
-        <v>309</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>33</v>
+        <v>407</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>474</v>
+        <v>408</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>475</v>
+        <v>409</v>
       </c>
       <c r="P22" s="16" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>114</v>
+        <v>256</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>115</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>116</v>
+        <v>495</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>117</v>
+        <v>379</v>
       </c>
       <c r="F23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="O23" s="12" t="s">
+        <v>501</v>
+      </c>
+      <c r="P23" s="16" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H23" s="2" t="s">
+      <c r="G24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="O23" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="I24" t="s">
-        <v>206</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>318</v>
+      <c r="I24" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>472</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>309</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N24" t="s">
-        <v>207</v>
+      <c r="N24" s="7" t="s">
+        <v>473</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>474</v>
+      </c>
+      <c r="P24" s="16" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
-        <v>448</v>
+        <v>114</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>449</v>
+        <v>116</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>379</v>
+        <v>117</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>451</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>46</v>
+        <v>118</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>453</v>
+        <v>326</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N25" t="s">
-        <v>454</v>
-      </c>
-      <c r="O25" s="7" t="s">
-        <v>455</v>
+        <v>31</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>456</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>129</v>
+        <v>201</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>131</v>
+        <v>203</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>117</v>
+        <v>176</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>132</v>
+        <v>204</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>167</v>
+        <v>466</v>
+      </c>
+      <c r="I26" t="s">
+        <v>206</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>343</v>
+        <v>317</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>327</v>
+        <v>21</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>344</v>
+        <v>318</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N26" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>133</v>
+        <v>208</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>233</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>430</v>
+        <v>448</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>431</v>
+        <v>130</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>432</v>
+        <v>449</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>379</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>118</v>
+        <v>450</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>433</v>
-      </c>
-      <c r="I27" s="16"/>
+        <v>451</v>
+      </c>
       <c r="J27" s="16" t="s">
-        <v>434</v>
-      </c>
-      <c r="K27" s="16" t="s">
-        <v>435</v>
+        <v>46</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>452</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>438</v>
-      </c>
-      <c r="M27" s="16" t="s">
-        <v>31</v>
+        <v>453</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="N27" t="s">
-        <v>436</v>
+        <v>454</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>437</v>
-      </c>
-      <c r="P27" s="16" t="s">
-        <v>439</v>
+        <v>455</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>395</v>
+        <v>129</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>396</v>
+        <v>130</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>397</v>
+        <v>131</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>379</v>
+        <v>117</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>227</v>
+        <v>132</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>398</v>
+        <v>343</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>399</v>
+        <v>327</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>400</v>
+        <v>344</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="N28" t="s">
-        <v>401</v>
+        <v>156</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>402</v>
-      </c>
-      <c r="P28" s="16" t="s">
-        <v>403</v>
+        <v>133</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
       <c r="B29" s="2" t="s">
-        <v>145</v>
+        <v>430</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>146</v>
+        <v>431</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>147</v>
+        <v>432</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>117</v>
+        <v>379</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>350</v>
+        <v>118</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>433</v>
+      </c>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="K29" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="L29" s="16" t="s">
+        <v>438</v>
+      </c>
+      <c r="M29" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N29" t="s">
+        <v>436</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="P29" s="16" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
-        <v>264</v>
+        <v>395</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>265</v>
+        <v>396</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>267</v>
+        <v>397</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>242</v>
+        <v>379</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>274</v>
+        <v>227</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>467</v>
+        <v>36</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>365</v>
+        <v>108</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>366</v>
+        <v>398</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>367</v>
+        <v>399</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>368</v>
+        <v>400</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="N30" t="s">
-        <v>268</v>
+        <v>401</v>
       </c>
       <c r="O30" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="P30" s="2" t="s">
-        <v>270</v>
+        <v>402</v>
+      </c>
+      <c r="P30" s="16" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="2" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>117</v>
@@ -3394,562 +3441,565 @@
         <v>27</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>55</v>
+        <v>148</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>237</v>
+        <v>24</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>46</v>
+        <v>347</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>369</v>
+        <v>348</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>21</v>
+        <v>349</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="O31" s="5" t="s">
-        <v>137</v>
+        <v>39</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
       <c r="B32" s="2" t="s">
-        <v>306</v>
+        <v>264</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>311</v>
+        <v>265</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>312</v>
+        <v>267</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>242</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>313</v>
+        <v>274</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>19</v>
+        <v>467</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>40</v>
+        <v>365</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>314</v>
+        <v>366</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>309</v>
+        <v>368</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N32" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="O32" s="2" t="s">
-        <v>307</v>
+        <v>31</v>
+      </c>
+      <c r="N32" t="s">
+        <v>268</v>
+      </c>
+      <c r="O32" s="7" t="s">
+        <v>269</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>308</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="2" t="s">
-        <v>486</v>
+        <v>134</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>487</v>
+        <v>135</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>488</v>
+        <v>136</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>379</v>
+        <v>117</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>489</v>
+        <v>55</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="2"/>
+      <c r="I33" s="2" t="s">
+        <v>237</v>
+      </c>
       <c r="J33" s="2" t="s">
-        <v>490</v>
+        <v>46</v>
       </c>
       <c r="K33" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="L33" s="16" t="s">
-        <v>491</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N33" s="12" t="s">
-        <v>492</v>
-      </c>
-      <c r="O33" s="12" t="s">
-        <v>493</v>
+      <c r="N33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="O33" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>494</v>
+        <v>342</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="2" t="s">
-        <v>64</v>
+        <v>306</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>240</v>
+        <v>311</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>241</v>
+        <v>312</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>242</v>
       </c>
       <c r="F34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+      <c r="B35" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="O34" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="P34" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
-        <v>44396.994444444441</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="G35" s="2" t="s">
-        <v>34</v>
+        <v>488</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>239</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>168</v>
+        <v>489</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>50</v>
+        <v>21</v>
+      </c>
+      <c r="L35" s="16" t="s">
+        <v>490</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N35" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="O35" s="5" t="s">
-        <v>52</v>
+        <v>22</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="O35" s="12" t="s">
+        <v>492</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="2" t="s">
-        <v>150</v>
+        <v>64</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>151</v>
+        <v>240</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>152</v>
+        <v>241</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>117</v>
+        <v>242</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
         <v>46</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>363</v>
+        <v>276</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>359</v>
+        <v>244</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N36" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="O36" s="2" t="s">
-        <v>154</v>
+        <v>20</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>44396.994444444441</v>
+      </c>
       <c r="B37" s="2" t="s">
-        <v>420</v>
+        <v>47</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>421</v>
+        <v>48</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>422</v>
+        <v>49</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>379</v>
+        <v>45</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>423</v>
+        <v>34</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I37" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="J37" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="K37" s="16" t="s">
-        <v>425</v>
+        <v>168</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>328</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>426</v>
+        <v>50</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N37" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="O37" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="P37" s="16" t="s">
-        <v>427</v>
+        <v>20</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="O37" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
-        <v>385</v>
+        <v>150</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>386</v>
+        <v>151</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>387</v>
+        <v>152</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>379</v>
+        <v>117</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>388</v>
+        <v>153</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="K38" s="16" t="s">
-        <v>390</v>
+        <v>46</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>363</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>391</v>
+        <v>359</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="O38" s="12" t="s">
-        <v>393</v>
+        <v>161</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="2" t="s">
-        <v>280</v>
+        <v>420</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>281</v>
+        <v>421</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>286</v>
+        <v>422</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>242</v>
+        <v>379</v>
       </c>
       <c r="F39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="K39" s="16" t="s">
+        <v>425</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="O39" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="P39" s="16" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+      <c r="B40" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="O39" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="P39" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
-        <v>44409.992361111108</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="G40" s="2" t="s">
-        <v>42</v>
+        <v>388</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>329</v>
+        <v>389</v>
+      </c>
+      <c r="K40" s="16" t="s">
+        <v>390</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>21</v>
+        <v>391</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="O40" s="2" t="s">
-        <v>75</v>
+        <v>394</v>
+      </c>
+      <c r="O40" s="12" t="s">
+        <v>393</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>170</v>
+        <v>392</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>242</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I41" s="2"/>
+      <c r="I41" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="J41" s="2" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>351</v>
+        <v>21</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>292</v>
+        <v>355</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N41" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="O41" s="2" t="s">
-        <v>294</v>
+        <v>35</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>284</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <v>44409.992361111108</v>
+      </c>
       <c r="B42" s="2" t="s">
-        <v>181</v>
+        <v>71</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>182</v>
+        <v>73</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>176</v>
+        <v>54</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="I42" t="s">
-        <v>183</v>
-      </c>
-      <c r="J42" s="11" t="s">
-        <v>184</v>
+        <v>42</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="L42" s="11" t="s">
-        <v>335</v>
+        <v>329</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N42" t="s">
-        <v>186</v>
-      </c>
-      <c r="O42" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="P42" s="13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>257</v>
+        <v>41</v>
+      </c>
+      <c r="N42" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+      <c r="B43" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>258</v>
+        <v>289</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>242</v>
@@ -3957,290 +4007,386 @@
       <c r="F43" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G43" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="K43" s="11" t="s">
-        <v>374</v>
-      </c>
-      <c r="L43" s="13" t="s">
-        <v>260</v>
+      <c r="G43" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>292</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N43" t="s">
-        <v>261</v>
-      </c>
-      <c r="O43" s="12" t="s">
-        <v>262</v>
+        <v>41</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>294</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="15">
-        <v>44397.036111111112</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>58</v>
+        <v>293</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>59</v>
+        <v>182</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>45</v>
+        <v>176</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G44" s="11" t="s">
-        <v>60</v>
+      <c r="G44" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>29</v>
+        <v>107</v>
+      </c>
+      <c r="I44" t="s">
+        <v>183</v>
       </c>
       <c r="J44" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K44" s="11" t="s">
-        <v>330</v>
+        <v>184</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>334</v>
       </c>
       <c r="L44" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M44" s="11" t="s">
-        <v>20</v>
+        <v>335</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="N44" t="s">
-        <v>61</v>
-      </c>
-      <c r="O44" s="14" t="s">
-        <v>62</v>
+        <v>186</v>
+      </c>
+      <c r="O44" s="12" t="s">
+        <v>187</v>
       </c>
       <c r="P44" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="15">
-        <v>44411.775694444441</v>
-      </c>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>77</v>
+        <v>256</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>257</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>78</v>
+        <v>258</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>54</v>
+        <v>242</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="H45" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="H45" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I45" s="2"/>
+      <c r="I45" s="11"/>
       <c r="J45" s="11" t="s">
-        <v>38</v>
+        <v>373</v>
       </c>
       <c r="K45" s="11" t="s">
-        <v>331</v>
+        <v>374</v>
       </c>
       <c r="L45" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="M45" s="11" t="s">
-        <v>56</v>
+        <v>260</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="N45" t="s">
-        <v>80</v>
-      </c>
-      <c r="O45" s="14" t="s">
-        <v>81</v>
+        <v>261</v>
+      </c>
+      <c r="O45" s="12" t="s">
+        <v>262</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>82</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>77</v>
+      <c r="A46" s="15">
+        <v>44397.036111111112</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>226</v>
+        <v>59</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>176</v>
+        <v>45</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>227</v>
+        <v>60</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="I46" t="s">
-        <v>183</v>
+        <v>29</v>
       </c>
       <c r="J46" s="11" t="s">
-        <v>345</v>
+        <v>30</v>
       </c>
       <c r="K46" s="11" t="s">
-        <v>238</v>
+        <v>330</v>
       </c>
       <c r="L46" s="11" t="s">
-        <v>228</v>
+        <v>28</v>
       </c>
       <c r="M46" s="11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N46" t="s">
-        <v>229</v>
-      </c>
-      <c r="O46" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="2" t="s">
-        <v>411</v>
+        <v>61</v>
+      </c>
+      <c r="O46" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="P46" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="15">
+        <v>44411.775694444441</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>412</v>
+        <v>77</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>413</v>
+        <v>78</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>379</v>
+        <v>54</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>414</v>
+        <v>79</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="J47" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="K47" s="16" t="s">
-        <v>416</v>
-      </c>
-      <c r="L47" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="I47" s="2"/>
+      <c r="J47" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K47" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="M47" s="11" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="N47" t="s">
-        <v>417</v>
-      </c>
-      <c r="O47" s="12" t="s">
-        <v>418</v>
+        <v>80</v>
+      </c>
+      <c r="O47" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="15">
-        <v>44405.647916666669</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>90</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>92</v>
+        <v>226</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>45</v>
+        <v>176</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G48" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="I48" t="s">
+        <v>183</v>
+      </c>
+      <c r="J48" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="K48" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="L48" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="M48" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N48" t="s">
+        <v>229</v>
+      </c>
+      <c r="O48" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="H49" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="J49" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="K49" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="L49" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M49" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N49" t="s">
+        <v>417</v>
+      </c>
+      <c r="O49" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="15">
+        <v>44405.647916666669</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="H50" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="J48" s="11" t="s">
+      <c r="J50" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K48" s="11" t="s">
+      <c r="K50" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="L48" s="13" t="s">
+      <c r="L50" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="M48" s="11" t="s">
+      <c r="M50" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="N48" t="s">
+      <c r="N50" t="s">
         <v>95</v>
       </c>
-      <c r="O48" s="12" t="s">
+      <c r="O50" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="P48" s="2" t="s">
+      <c r="P50" s="2" t="s">
         <v>362</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:P41">
-    <sortCondition ref="C3:C41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:P43">
+    <sortCondition ref="C3:C43"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="N32" r:id="rId1" xr:uid="{CBF3488F-0731-4784-B778-22BEDC9A87FD}"/>
+    <hyperlink ref="N34" r:id="rId1" xr:uid="{CBF3488F-0731-4784-B778-22BEDC9A87FD}"/>
     <hyperlink ref="O5" r:id="rId2" xr:uid="{AA553A20-924A-4A7A-B3C1-6D6F29D53AB7}"/>
-    <hyperlink ref="O38" r:id="rId3" xr:uid="{9F78E4A3-9753-40AC-9C13-EFA682AF983E}"/>
-    <hyperlink ref="O28" r:id="rId4" xr:uid="{C0B53B11-AD93-46B5-9A27-594CC3A5271C}"/>
-    <hyperlink ref="N21" r:id="rId5" xr:uid="{19C35423-B41E-431E-A7D2-61DD10A2F89A}"/>
-    <hyperlink ref="O21" r:id="rId6" xr:uid="{FE29F50A-8A83-4CCD-A9E1-9EC92A26530E}"/>
-    <hyperlink ref="O47" r:id="rId7" xr:uid="{365E22B1-13F2-4C32-B64B-BC5B771A124E}"/>
-    <hyperlink ref="O37" r:id="rId8" xr:uid="{EE808F38-5A70-43A7-B847-4DFEFF8C2345}"/>
-    <hyperlink ref="O27" r:id="rId9" xr:uid="{C7957FDB-9E17-4A60-BBEB-6ACA89C74CF0}"/>
-    <hyperlink ref="O17" r:id="rId10" xr:uid="{F34024D8-C79C-4E14-91EB-C1D38E6B185F}"/>
-    <hyperlink ref="O25" r:id="rId11" xr:uid="{A8E15ABD-7D2B-4B1E-90AD-87A935FE52C9}"/>
+    <hyperlink ref="O40" r:id="rId3" xr:uid="{9F78E4A3-9753-40AC-9C13-EFA682AF983E}"/>
+    <hyperlink ref="O30" r:id="rId4" xr:uid="{C0B53B11-AD93-46B5-9A27-594CC3A5271C}"/>
+    <hyperlink ref="N22" r:id="rId5" xr:uid="{19C35423-B41E-431E-A7D2-61DD10A2F89A}"/>
+    <hyperlink ref="O22" r:id="rId6" xr:uid="{FE29F50A-8A83-4CCD-A9E1-9EC92A26530E}"/>
+    <hyperlink ref="O49" r:id="rId7" xr:uid="{365E22B1-13F2-4C32-B64B-BC5B771A124E}"/>
+    <hyperlink ref="O39" r:id="rId8" xr:uid="{EE808F38-5A70-43A7-B847-4DFEFF8C2345}"/>
+    <hyperlink ref="O29" r:id="rId9" xr:uid="{C7957FDB-9E17-4A60-BBEB-6ACA89C74CF0}"/>
+    <hyperlink ref="O18" r:id="rId10" xr:uid="{F34024D8-C79C-4E14-91EB-C1D38E6B185F}"/>
+    <hyperlink ref="O27" r:id="rId11" xr:uid="{A8E15ABD-7D2B-4B1E-90AD-87A935FE52C9}"/>
     <hyperlink ref="O2" r:id="rId12" xr:uid="{9EFE127E-94E1-4D1A-B4FF-56A0D7F365F6}"/>
-    <hyperlink ref="O22" r:id="rId13" xr:uid="{694135F8-96D1-41DA-A6C7-782217CF8081}"/>
-    <hyperlink ref="O20" r:id="rId14" xr:uid="{4AFEC0A6-99D6-4CB4-AA7F-2747B52DE82F}"/>
-    <hyperlink ref="O33" r:id="rId15" xr:uid="{1CF56EA4-06F0-461F-9648-39BB0DCA36A3}"/>
+    <hyperlink ref="O24" r:id="rId13" xr:uid="{694135F8-96D1-41DA-A6C7-782217CF8081}"/>
+    <hyperlink ref="O21" r:id="rId14" xr:uid="{4AFEC0A6-99D6-4CB4-AA7F-2747B52DE82F}"/>
+    <hyperlink ref="O35" r:id="rId15" xr:uid="{1CF56EA4-06F0-461F-9648-39BB0DCA36A3}"/>
+    <hyperlink ref="N23" r:id="rId16" xr:uid="{59E4A675-78BA-4241-9770-4D060595A68E}"/>
+    <hyperlink ref="O23" r:id="rId17" xr:uid="{3A71C51C-0184-4AC7-AFF4-DD100418FA0C}"/>
+    <hyperlink ref="N11" r:id="rId18" xr:uid="{DFD50037-4AF8-4266-B9E8-32F987D61850}"/>
+    <hyperlink ref="O11" r:id="rId19" xr:uid="{5DDFB26C-A00E-4DCD-860F-446A67100756}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId16"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed typo in Abigail bio
</commit_message>
<xml_diff>
--- a/src/data/summerfall23/bios_summerfall23.xlsx
+++ b/src/data/summerfall23/bios_summerfall23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abigailbareiss/dspuci-website-gatsby/src/data/summerfall23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1979607E-7827-D945-8E2B-D7B6535D5C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978738C2-802D-7949-8313-B370E6073E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="760" windowWidth="22460" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1558,7 +1558,7 @@
     <t>Hi hi! My name is Alli, and I initiated spring of my second year with the Alpha Omicron class. In my free time, I love to dance, snowboard, go to the beach, and travel. A fun fact is that I have a deadly phobia of snails! Feel free to ask me about my favorite TV shows to binge watch, and why elephants are the best animals in the world — I can't wait to meet everyone!</t>
   </si>
   <si>
-    <t xml:space="preserve">Hello I'm Abigail! I initiated in the spring of my sophomore year with the Alpha Omicron class. In my free time, I enjoy hiking, baking, doing yoga, singing, and thrifting! Ask me about my my favorite traveling adventures or anything else during recruitment! </t>
+    <t xml:space="preserve">Hi I'm Abigail! I initiated in the spring of my sophomore year with the Alpha Omicron class. In my free time, I enjoy hiking, baking, doing yoga, singing, and thrifting! Ask me about my favorite traveling adventures or anything else during recruitment! </t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added president letter and chapter pic
</commit_message>
<xml_diff>
--- a/src/data/summerfall23/bios_summerfall23.xlsx
+++ b/src/data/summerfall23/bios_summerfall23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abigailbareiss/dspuci-website-gatsby/src/data/summerfall23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978738C2-802D-7949-8313-B370E6073E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4437D0B8-1CFF-9645-85FA-723220F2A7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="760" windowWidth="22460" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2001,7 +2001,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P5" sqref="P5"/>
+      <selection pane="bottomRight" activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
F'23 Recruitment page and major updates
</commit_message>
<xml_diff>
--- a/src/data/summerfall23/bios_summerfall23.xlsx
+++ b/src/data/summerfall23/bios_summerfall23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abigailbareiss/dspuci-website-gatsby/src/data/summerfall23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4437D0B8-1CFF-9645-85FA-723220F2A7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D03EA2-7FFD-E140-8388-4BA0DE420A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="760" windowWidth="22460" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="760" windowWidth="26160" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -1015,9 +1015,6 @@
     <t>Software Developer @ LinQuest</t>
   </si>
   <si>
-    <t>HR Intern @ Kaiser Permanente</t>
-  </si>
-  <si>
     <t>SPFB</t>
   </si>
   <si>
@@ -1559,13 +1556,16 @@
   </si>
   <si>
     <t xml:space="preserve">Hi I'm Abigail! I initiated in the spring of my sophomore year with the Alpha Omicron class. In my free time, I enjoy hiking, baking, doing yoga, singing, and thrifting! Ask me about my favorite traveling adventures or anything else during recruitment! </t>
+  </si>
+  <si>
+    <t>HR Shared Services Intern @ Proofpoint, Inc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1998,13 +1998,13 @@
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R5" sqref="R5"/>
+      <selection pane="bottomRight" activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
@@ -2021,7 +2021,7 @@
     <col min="15" max="23" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13">
+    <row r="1" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2071,53 +2071,53 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13">
+    <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>458</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="L2" s="16" t="s">
         <v>460</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>461</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>462</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="13">
+    </row>
+    <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>44404.515972222223</v>
       </c>
@@ -2146,13 +2146,13 @@
         <v>108</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>353</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>354</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>41</v>
@@ -2167,7 +2167,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="13">
+    <row r="4" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
         <v>196</v>
       </c>
@@ -2193,13 +2193,13 @@
         <v>40</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>337</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>41</v>
@@ -2214,24 +2214,24 @@
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>379</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>29</v>
@@ -2243,22 +2243,22 @@
         <v>21</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="N5" t="s">
+        <v>381</v>
+      </c>
+      <c r="O5" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="O5" s="12" t="s">
-        <v>383</v>
-      </c>
       <c r="P5" s="16" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="13">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>44404.857638888891</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="13">
+    <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
         <v>248</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>253</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>20</v>
@@ -2351,7 +2351,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="13">
+    <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
         <v>218</v>
       </c>
@@ -2377,10 +2377,10 @@
         <v>221</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>222</v>
@@ -2395,10 +2395,10 @@
         <v>224</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="13">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
         <v>173</v>
       </c>
@@ -2421,16 +2421,16 @@
         <v>36</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>179</v>
       </c>
       <c r="K9" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>339</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>16</v>
@@ -2445,7 +2445,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="13">
+    <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
         <v>188</v>
@@ -2493,54 +2493,54 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1">
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>503</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>37</v>
       </c>
       <c r="I11" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="J11" s="11" t="s">
         <v>505</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="K11" s="11" t="s">
         <v>506</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="L11" s="11" t="s">
         <v>507</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>508</v>
       </c>
       <c r="M11" s="11" t="s">
         <v>26</v>
       </c>
       <c r="N11" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="O11" s="14" t="s">
         <v>509</v>
       </c>
-      <c r="O11" s="14" t="s">
+      <c r="P11" s="11" t="s">
         <v>510</v>
       </c>
-      <c r="P11" s="11" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="13">
+    </row>
+    <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>44404.652777777781</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="13">
+    <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="15">
         <v>44397.381944444445</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>172</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>316</v>
@@ -2638,7 +2638,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="13">
+    <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B14" s="2" t="s">
         <v>271</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="14.25" customHeight="1">
+    <row r="15" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
         <v>209</v>
@@ -2707,7 +2707,7 @@
         <v>119</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>213</v>
@@ -2731,7 +2731,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15">
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="15">
         <v>44397.802083333336</v>
       </c>
@@ -2757,16 +2757,16 @@
         <v>19</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J16" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>358</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>39</v>
@@ -2781,7 +2781,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="13">
+    <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
         <v>138</v>
@@ -2827,19 +2827,19 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="13">
+    <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>441</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>14</v>
@@ -2852,28 +2852,28 @@
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>33</v>
       </c>
       <c r="N18" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="O18" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="O18" s="7" t="s">
+      <c r="P18" s="16" t="s">
         <v>445</v>
       </c>
-      <c r="P18" s="16" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="14">
+    </row>
+    <row r="19" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="2" t="s">
         <v>123</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>321</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L19" s="10" t="s">
         <v>322</v>
@@ -2920,7 +2920,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="13">
+    <row r="20" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
         <v>296</v>
       </c>
@@ -2965,75 +2965,75 @@
         <v>303</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="13">
+    <row r="21" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>477</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J21" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="K21" s="16" t="s">
         <v>478</v>
       </c>
-      <c r="K21" s="16" t="s">
+      <c r="L21" s="16" t="s">
         <v>479</v>
-      </c>
-      <c r="L21" s="16" t="s">
-        <v>480</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>41</v>
       </c>
       <c r="N21" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="O21" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="O21" s="7" t="s">
+      <c r="P21" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15">
+    </row>
+    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.15">
       <c r="B22" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>115</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>119</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="16" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>21</v>
@@ -3045,16 +3045,16 @@
         <v>25</v>
       </c>
       <c r="N22" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="O22" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="O22" s="7" t="s">
+      <c r="P22" s="16" t="s">
         <v>408</v>
       </c>
-      <c r="P22" s="16" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1">
+    </row>
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="2" t="s">
         <v>256</v>
       </c>
@@ -3062,54 +3062,54 @@
         <v>115</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K23" s="11" t="s">
         <v>21</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N23" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="O23" s="12" t="s">
         <v>499</v>
       </c>
-      <c r="O23" s="12" t="s">
-        <v>500</v>
-      </c>
       <c r="P23" s="16" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="13">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B24" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>115</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>27</v>
@@ -3121,13 +3121,13 @@
         <v>119</v>
       </c>
       <c r="I24" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="J24" s="16" t="s">
         <v>469</v>
       </c>
-      <c r="J24" s="16" t="s">
+      <c r="K24" s="16" t="s">
         <v>470</v>
-      </c>
-      <c r="K24" s="16" t="s">
-        <v>471</v>
       </c>
       <c r="L24" s="16" t="s">
         <v>309</v>
@@ -3136,16 +3136,16 @@
         <v>33</v>
       </c>
       <c r="N24" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="O24" s="7" t="s">
         <v>472</v>
       </c>
-      <c r="O24" s="7" t="s">
+      <c r="P24" s="16" t="s">
         <v>473</v>
       </c>
-      <c r="P24" s="16" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="13">
+    </row>
+    <row r="25" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
         <v>114</v>
@@ -3193,7 +3193,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15.75" customHeight="1">
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="2" t="s">
         <v>201</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>204</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I26" t="s">
         <v>206</v>
@@ -3240,51 +3240,51 @@
         <v>319</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1">
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="H27" s="16" t="s">
         <v>449</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>450</v>
       </c>
       <c r="J27" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K27" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="L27" s="16" t="s">
         <v>451</v>
-      </c>
-      <c r="L27" s="16" t="s">
-        <v>452</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N27" t="s">
+        <v>452</v>
+      </c>
+      <c r="O27" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="O27" s="7" t="s">
+      <c r="P27" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="P27" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1">
+    </row>
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="2" t="s">
         <v>129</v>
       </c>
@@ -3310,13 +3310,13 @@
         <v>167</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>327</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>31</v>
@@ -3331,18 +3331,18 @@
         <v>233</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>431</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>27</v>
@@ -3351,43 +3351,43 @@
         <v>118</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I29" s="16"/>
       <c r="J29" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="K29" s="16" t="s">
         <v>433</v>
       </c>
-      <c r="K29" s="16" t="s">
-        <v>434</v>
-      </c>
       <c r="L29" s="16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="M29" s="16" t="s">
         <v>31</v>
       </c>
       <c r="N29" t="s">
+        <v>434</v>
+      </c>
+      <c r="O29" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="O29" s="7" t="s">
-        <v>436</v>
-      </c>
       <c r="P29" s="16" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>396</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>27</v>
@@ -3402,28 +3402,28 @@
         <v>108</v>
       </c>
       <c r="J30" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="L30" s="2" t="s">
         <v>398</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>399</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N30" t="s">
+        <v>399</v>
+      </c>
+      <c r="O30" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="O30" s="7" t="s">
+      <c r="P30" s="16" t="s">
         <v>401</v>
       </c>
-      <c r="P30" s="16" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1">
+    </row>
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="2" t="s">
         <v>145</v>
@@ -3450,13 +3450,13 @@
         <v>104</v>
       </c>
       <c r="J31" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="K31" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="L31" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>349</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>39</v>
@@ -3468,10 +3468,10 @@
         <v>149</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="15.75" customHeight="1">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="2" t="s">
         <v>264</v>
       </c>
@@ -3491,19 +3491,19 @@
         <v>274</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I32" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="K32" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="L32" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>368</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>31</v>
@@ -3518,7 +3518,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="15.75" customHeight="1">
+    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="B33" s="2" t="s">
         <v>134</v>
@@ -3548,7 +3548,7 @@
         <v>46</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>21</v>
@@ -3563,10 +3563,10 @@
         <v>137</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" ht="15.75" customHeight="1">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="2" t="s">
         <v>306</v>
@@ -3605,7 +3605,7 @@
         <v>22</v>
       </c>
       <c r="N34" s="12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O34" s="2" t="s">
         <v>307</v>
@@ -3614,53 +3614,53 @@
         <v>308</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="15.75" customHeight="1">
+    <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="B35" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>486</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L35" s="16" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N35" s="12" t="s">
+        <v>489</v>
+      </c>
+      <c r="O35" s="12" t="s">
         <v>490</v>
       </c>
-      <c r="O35" s="12" t="s">
+      <c r="P35" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="P35" s="2" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" ht="15.75" customHeight="1">
+    </row>
+    <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="2" t="s">
         <v>64</v>
@@ -3706,7 +3706,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="15.75" customHeight="1">
+    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
         <v>44396.994444444441</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="15" customHeight="1">
+    <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
         <v>150</v>
@@ -3784,10 +3784,10 @@
         <v>46</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>33</v>
@@ -3802,99 +3802,99 @@
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="15" customHeight="1">
+    <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>421</v>
-      </c>
       <c r="E39" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="K39" s="16" t="s">
         <v>423</v>
       </c>
-      <c r="K39" s="16" t="s">
+      <c r="L39" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>425</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="O39" s="12" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P39" s="16" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="15" customHeight="1">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>386</v>
-      </c>
       <c r="E40" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K40" s="16" t="s">
         <v>388</v>
       </c>
-      <c r="K40" s="16" t="s">
+      <c r="L40" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>390</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>35</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="O40" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="15.75" customHeight="1">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="2" t="s">
         <v>280</v>
@@ -3927,7 +3927,7 @@
         <v>21</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>35</v>
@@ -3942,7 +3942,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="15.75" customHeight="1">
+    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3">
         <v>44409.992361111108</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="15.75" customHeight="1">
+    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="3"/>
       <c r="B43" s="2" t="s">
         <v>287</v>
@@ -4018,7 +4018,7 @@
         <v>291</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>292</v>
@@ -4036,7 +4036,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="15.75" customHeight="1">
+    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>181</v>
       </c>
@@ -4065,10 +4065,10 @@
         <v>184</v>
       </c>
       <c r="K44" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="L44" s="11" t="s">
         <v>334</v>
-      </c>
-      <c r="L44" s="11" t="s">
-        <v>335</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>33</v>
@@ -4083,7 +4083,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15.75" customHeight="1">
+    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="11" t="s">
         <v>256</v>
       </c>
@@ -4107,10 +4107,10 @@
       </c>
       <c r="I45" s="11"/>
       <c r="J45" s="11" t="s">
+        <v>372</v>
+      </c>
+      <c r="K45" s="11" t="s">
         <v>373</v>
-      </c>
-      <c r="K45" s="11" t="s">
-        <v>374</v>
       </c>
       <c r="L45" s="13" t="s">
         <v>260</v>
@@ -4128,7 +4128,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="15.75" customHeight="1">
+    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="15">
         <v>44397.036111111112</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="15.75" customHeight="1">
+    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15">
         <v>44411.775694444441</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>38</v>
       </c>
       <c r="K47" s="11" t="s">
-        <v>331</v>
+        <v>512</v>
       </c>
       <c r="L47" s="13" t="s">
         <v>28</v>
@@ -4223,7 +4223,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="15.75" customHeight="1">
+    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="2" t="s">
         <v>225</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>183</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K48" s="11" t="s">
         <v>238</v>
@@ -4270,33 +4270,33 @@
         <v>231</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="15.75" customHeight="1">
+    <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>412</v>
-      </c>
       <c r="E49" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G49" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="H49" s="11" t="s">
         <v>413</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>414</v>
       </c>
       <c r="J49" s="16" t="s">
         <v>109</v>
       </c>
       <c r="K49" s="16" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L49" s="11" t="s">
         <v>21</v>
@@ -4305,16 +4305,16 @@
         <v>26</v>
       </c>
       <c r="N49" t="s">
+        <v>415</v>
+      </c>
+      <c r="O49" s="12" t="s">
         <v>416</v>
       </c>
-      <c r="O49" s="12" t="s">
+      <c r="P49" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="P49" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="15.75" customHeight="1">
+    </row>
+    <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="15">
         <v>44405.647916666669</v>
       </c>
@@ -4343,10 +4343,10 @@
         <v>94</v>
       </c>
       <c r="K50" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="L50" s="13" t="s">
         <v>360</v>
-      </c>
-      <c r="L50" s="13" t="s">
-        <v>361</v>
       </c>
       <c r="M50" s="11" t="s">
         <v>31</v>
@@ -4358,7 +4358,7 @@
         <v>96</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Diana bio and removed inactive bros
</commit_message>
<xml_diff>
--- a/src/data/summerfall23/bios_summerfall23.xlsx
+++ b/src/data/summerfall23/bios_summerfall23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abigailbareiss/dspuci-website-gatsby/src/data/summerfall23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62841915-1102-1547-AC22-FD5C6335A8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC665B75-0225-374A-BFF5-4AA58D56B348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="860" windowWidth="26160" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="495">
   <si>
     <t>Timestamp</t>
   </si>
@@ -334,9 +334,6 @@
     <t>Hello! My name is Sean Devine and I initiated in the spring quarter of my first year here at UCI. In my free time, I enjoy any form of sport and competition. Currently, I am learning how to surf. Ask me about stocks, favorite books, and Formula 1 at recruitment!</t>
   </si>
   <si>
-    <t>Psychological Science</t>
-  </si>
-  <si>
     <t>Truong</t>
   </si>
   <si>
@@ -457,21 +454,6 @@
     <t>Hi! My name is Jason Henkel and I initiated during the fall of my first year with the Alpha Mu class. Outside of school, I love playing sports, trying new things, and exploring new areas. Ask me about my NBA predictions or favorite movies at recruitment!</t>
   </si>
   <si>
-    <t>Elin</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>elin_min</t>
-  </si>
-  <si>
-    <t>Seoul, South Korea</t>
-  </si>
-  <si>
-    <t>elinmin@ucidsp.com</t>
-  </si>
-  <si>
     <t>Winnie</t>
   </si>
   <si>
@@ -499,9 +481,6 @@
     <t>https://www.linkedin.com/in/jasonfhenkel/</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/elin-eunkee-min/</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/jakesmoss/</t>
   </si>
   <si>
@@ -859,27 +838,6 @@
     <t>https://www.linkedin.com/in/safahfaraz/</t>
   </si>
   <si>
-    <t>Sumin</t>
-  </si>
-  <si>
-    <t>Sung</t>
-  </si>
-  <si>
-    <t>Honolulu, HI</t>
-  </si>
-  <si>
-    <t>Hi! My name is Sumin, and I initiated with the Alpha Xi class during the fall quarter of my second year. In my free time, I enjoy thrifting, going to the beach, and trying new food spots with friends. Feel free to ask me about my favorite TV shows/movies, my travel bucket list, or anything else at recruitment :-)!</t>
-  </si>
-  <si>
-    <t>suminsung@ucidsp.com</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/suminsung/</t>
-  </si>
-  <si>
-    <t>sumin_sung</t>
-  </si>
-  <si>
     <t>Ai</t>
   </si>
   <si>
@@ -919,12 +877,6 @@
     <t>Laguna Hills, CA</t>
   </si>
   <si>
-    <t>Sports Business, Consulting, Marketing</t>
-  </si>
-  <si>
-    <t>Marketing Assistant @ UCI Athletics</t>
-  </si>
-  <si>
     <t>Sports Business Association, UCI Women’s Club Soccer</t>
   </si>
   <si>
@@ -1051,18 +1003,6 @@
     <t xml:space="preserve">Philosophy </t>
   </si>
   <si>
-    <t>Marketing, Human Resources</t>
-  </si>
-  <si>
-    <t>Educator/Marketing Intern @ Lululemon</t>
-  </si>
-  <si>
-    <t>HRMA</t>
-  </si>
-  <si>
-    <t>Hey! My name is Elin Min, and I initiated in Fall 2021 with the Alpha Mu Class. In my free time, I enjoy playing tennis and basketball, working out, listening to EDM, and going to raves. Feel free to ask me about my life in Thailand, Canada, and Korea at recruitment!</t>
-  </si>
-  <si>
     <t xml:space="preserve">Campus Leader @ Quokka Brew </t>
   </si>
   <si>
@@ -1075,9 +1015,6 @@
     <t xml:space="preserve">Latino Business Student Association , Merage Financial Service - Student Assistant, Sigma Chi Fraternity, UCI Athletics </t>
   </si>
   <si>
-    <t>MAISS, UCI Housing</t>
-  </si>
-  <si>
     <t>Digital Marketing, Marketing Strategy</t>
   </si>
   <si>
@@ -1562,6 +1499,12 @@
   </si>
   <si>
     <t>Finance Leadership Development Program @ Thermo Fisher Scientific, Student Assistant for MBA Recruitment and Administration @ The Paul Merage School of Business</t>
+  </si>
+  <si>
+    <t>Information Systems, Tech Consulting, Marketing</t>
+  </si>
+  <si>
+    <t>Data Analytics Inters @ General Atomics - ASI</t>
   </si>
 </sst>
 </file>
@@ -1998,13 +1941,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P50"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y19" sqref="Y19"/>
+      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2077,47 +2020,47 @@
     <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>450</v>
+        <v>429</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>451</v>
+        <v>430</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>452</v>
+        <v>431</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>453</v>
+        <v>432</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>487</v>
+        <v>466</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>507</v>
+        <v>486</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>454</v>
+        <v>433</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>455</v>
+        <v>434</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>456</v>
+        <v>435</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2143,19 +2086,19 @@
         <v>67</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>41</v>
@@ -2172,22 +2115,22 @@
     </row>
     <row r="4" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>19</v>
@@ -2196,45 +2139,45 @@
         <v>40</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>369</v>
+        <v>348</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>41</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="11" t="s">
-        <v>370</v>
+        <v>349</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>371</v>
+        <v>350</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>374</v>
+        <v>353</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>29</v>
@@ -2246,19 +2189,19 @@
         <v>21</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>375</v>
+        <v>354</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="N5" t="s">
-        <v>376</v>
+        <v>355</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>377</v>
+        <v>356</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2291,7 +2234,7 @@
         <v>30</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>86</v>
@@ -2311,108 +2254,108 @@
     </row>
     <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="M8" t="s">
         <v>20</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>367</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>18</v>
@@ -2424,43 +2367,43 @@
         <v>36</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>27</v>
@@ -2475,72 +2418,72 @@
         <v>40</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>513</v>
+        <v>492</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
-        <v>493</v>
+        <v>472</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>494</v>
+        <v>473</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>495</v>
+        <v>474</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>37</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>497</v>
+        <v>476</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>498</v>
+        <v>477</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
       <c r="M11" s="11" t="s">
         <v>26</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>502</v>
+        <v>481</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2570,13 +2513,13 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>35</v>
@@ -2596,63 +2539,63 @@
         <v>44397.381944444445</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>510</v>
+        <v>489</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B14" s="2" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>14</v>
@@ -2665,73 +2608,73 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="N14" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.15">
@@ -2739,13 +2682,13 @@
         <v>44397.802083333336</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>45</v>
@@ -2760,56 +2703,56 @@
         <v>19</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>352</v>
+        <v>331</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>353</v>
+        <v>332</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>354</v>
+        <v>333</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>39</v>
       </c>
       <c r="N16" t="s">
+        <v>111</v>
+      </c>
+      <c r="O16" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="O16" s="7" t="s">
-        <v>113</v>
-      </c>
       <c r="P16" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>21</v>
@@ -2821,28 +2764,28 @@
         <v>16</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="O17" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P17" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
-        <v>433</v>
+        <v>412</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>434</v>
+        <v>413</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>14</v>
@@ -2855,188 +2798,188 @@
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>436</v>
+        <v>415</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>437</v>
+        <v>416</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>33</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>438</v>
+        <v>417</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
       <c r="P18" s="16" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>485</v>
+        <v>464</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>35</v>
       </c>
       <c r="N19" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="O19" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="P19" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="E20" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>299</v>
+        <v>493</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>300</v>
+        <v>494</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
-        <v>467</v>
+        <v>446</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>468</v>
+        <v>447</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>469</v>
+        <v>448</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>381</v>
+        <v>360</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>470</v>
+        <v>449</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>471</v>
+        <v>450</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>41</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
       <c r="O21" s="7" t="s">
-        <v>474</v>
+        <v>453</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>475</v>
+        <v>454</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.15">
       <c r="B22" s="2" t="s">
-        <v>397</v>
+        <v>376</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>398</v>
+        <v>377</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>399</v>
+        <v>378</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="16" t="s">
-        <v>400</v>
+        <v>379</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>21</v>
@@ -3048,71 +2991,71 @@
         <v>25</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>401</v>
+        <v>380</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>402</v>
+        <v>381</v>
       </c>
       <c r="P22" s="16" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="2" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>486</v>
+        <v>465</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>479</v>
+        <v>458</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>488</v>
+        <v>467</v>
       </c>
       <c r="K23" s="11" t="s">
         <v>21</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>489</v>
+        <v>468</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>491</v>
+        <v>470</v>
       </c>
       <c r="O23" s="12" t="s">
-        <v>492</v>
+        <v>471</v>
       </c>
       <c r="P23" s="16" t="s">
-        <v>490</v>
+        <v>469</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B24" s="2" t="s">
-        <v>459</v>
+        <v>438</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>460</v>
+        <v>439</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>27</v>
@@ -3121,1269 +3064,1173 @@
         <v>15</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>461</v>
+        <v>440</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>33</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>464</v>
+        <v>443</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>465</v>
+        <v>444</v>
       </c>
       <c r="P24" s="16" t="s">
-        <v>466</v>
+        <v>445</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>40</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>31</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="2" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>457</v>
+        <v>436</v>
       </c>
       <c r="I26" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>33</v>
       </c>
       <c r="N26" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="2" t="s">
-        <v>441</v>
+        <v>420</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>442</v>
+        <v>421</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>443</v>
+        <v>422</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>444</v>
+        <v>423</v>
       </c>
       <c r="J27" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>445</v>
+        <v>424</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>446</v>
+        <v>425</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N27" t="s">
-        <v>447</v>
+        <v>426</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>448</v>
+        <v>427</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>449</v>
+        <v>428</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>31</v>
       </c>
       <c r="N28" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="2" t="s">
-        <v>423</v>
+        <v>402</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>425</v>
+        <v>404</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>426</v>
+        <v>405</v>
       </c>
       <c r="I29" s="16"/>
       <c r="J29" s="16" t="s">
-        <v>427</v>
+        <v>406</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
       <c r="L29" s="16" t="s">
-        <v>431</v>
+        <v>410</v>
       </c>
       <c r="M29" s="16" t="s">
         <v>31</v>
       </c>
       <c r="N29" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>430</v>
+        <v>409</v>
       </c>
       <c r="P29" s="16" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="2" t="s">
-        <v>388</v>
+        <v>367</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>389</v>
+        <v>368</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>391</v>
+        <v>370</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>392</v>
+        <v>371</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>393</v>
+        <v>372</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N30" t="s">
-        <v>394</v>
+        <v>373</v>
       </c>
       <c r="O30" s="7" t="s">
-        <v>395</v>
+        <v>374</v>
       </c>
       <c r="P30" s="16" t="s">
-        <v>396</v>
+        <v>375</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="3"/>
       <c r="B31" s="2" t="s">
-        <v>145</v>
+        <v>256</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>146</v>
+        <v>257</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>147</v>
+        <v>259</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>117</v>
+        <v>234</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>148</v>
+        <v>266</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>104</v>
+        <v>437</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>339</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N31" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>149</v>
+        <v>31</v>
+      </c>
+      <c r="N31" t="s">
+        <v>260</v>
+      </c>
+      <c r="O31" s="7" t="s">
+        <v>261</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>346</v>
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="3"/>
       <c r="B32" s="2" t="s">
-        <v>263</v>
+        <v>133</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>264</v>
+        <v>134</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>266</v>
+        <v>135</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>241</v>
+        <v>116</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>273</v>
+        <v>55</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>458</v>
+        <v>19</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>360</v>
+        <v>229</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>361</v>
+        <v>46</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>363</v>
+        <v>21</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N32" t="s">
-        <v>267</v>
-      </c>
-      <c r="O32" s="7" t="s">
-        <v>268</v>
+        <v>22</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>269</v>
+        <v>322</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="B33" s="2" t="s">
-        <v>134</v>
+        <v>289</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>135</v>
+        <v>293</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>136</v>
+        <v>294</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>117</v>
+        <v>234</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>55</v>
+        <v>295</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>236</v>
+        <v>40</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>46</v>
+        <v>296</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>364</v>
+        <v>488</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>21</v>
+        <v>292</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N33" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="O33" s="5" t="s">
-        <v>137</v>
+      <c r="N33" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>338</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="2" t="s">
-        <v>305</v>
+        <v>455</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>309</v>
+        <v>456</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>310</v>
+        <v>457</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>241</v>
+        <v>352</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>311</v>
+        <v>458</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="I34" s="2"/>
       <c r="J34" s="2" t="s">
-        <v>312</v>
+        <v>459</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>308</v>
+        <v>21</v>
+      </c>
+      <c r="L34" s="16" t="s">
+        <v>460</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N34" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>306</v>
+        <v>461</v>
+      </c>
+      <c r="O34" s="12" t="s">
+        <v>462</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>307</v>
+        <v>463</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="B35" s="2" t="s">
-        <v>476</v>
+        <v>64</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>477</v>
+        <v>232</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>478</v>
+        <v>233</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>373</v>
+        <v>234</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>479</v>
+        <v>235</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>480</v>
+        <v>46</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L35" s="16" t="s">
-        <v>481</v>
+        <v>268</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N35" s="12" t="s">
-        <v>482</v>
-      </c>
-      <c r="O35" s="12" t="s">
-        <v>483</v>
+        <v>20</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="O35" s="5" t="s">
+        <v>238</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>484</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="3"/>
+      <c r="A36" s="3">
+        <v>44396.994444444441</v>
+      </c>
       <c r="B36" s="2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>239</v>
+        <v>48</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>240</v>
+        <v>49</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>241</v>
+        <v>45</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>242</v>
+        <v>34</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I36" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>231</v>
+      </c>
       <c r="J36" s="2" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>275</v>
+        <v>310</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>243</v>
+        <v>50</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N36" s="1" t="s">
-        <v>244</v>
+      <c r="N36" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>245</v>
+        <v>52</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="3">
-        <v>44396.994444444441</v>
-      </c>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="3"/>
       <c r="B37" s="2" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>48</v>
+        <v>145</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>238</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="I37" s="2"/>
       <c r="J37" s="2" t="s">
-        <v>168</v>
+        <v>459</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>326</v>
+        <v>490</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>50</v>
+        <v>334</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N37" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="O37" s="5" t="s">
-        <v>52</v>
+        <v>33</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>53</v>
+        <v>491</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
-        <v>150</v>
+        <v>392</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>151</v>
+        <v>393</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>152</v>
+        <v>394</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>117</v>
+        <v>352</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>153</v>
+        <v>395</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>511</v>
+        <v>396</v>
+      </c>
+      <c r="K38" s="16" t="s">
+        <v>397</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>355</v>
+        <v>398</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="O38" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>512</v>
+        <v>401</v>
+      </c>
+      <c r="O38" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="P38" s="16" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="2" t="s">
-        <v>413</v>
+        <v>357</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>414</v>
+        <v>358</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>415</v>
+        <v>359</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>416</v>
+        <v>360</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2" t="s">
-        <v>417</v>
+        <v>361</v>
       </c>
       <c r="K39" s="16" t="s">
-        <v>418</v>
+        <v>362</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>419</v>
+        <v>363</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>422</v>
+        <v>366</v>
       </c>
       <c r="O39" s="12" t="s">
-        <v>421</v>
-      </c>
-      <c r="P39" s="16" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="3"/>
+        <v>365</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="3">
+        <v>44409.992361111108</v>
+      </c>
       <c r="B40" s="2" t="s">
-        <v>378</v>
+        <v>71</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>379</v>
+        <v>72</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>380</v>
+        <v>73</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>373</v>
+        <v>54</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>381</v>
+        <v>42</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="K40" s="16" t="s">
-        <v>383</v>
+        <v>108</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>384</v>
+        <v>21</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="O40" s="12" t="s">
-        <v>386</v>
+        <v>74</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>385</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>108</v>
-      </c>
+      <c r="I41" s="2"/>
       <c r="J41" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>21</v>
+        <v>327</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>351</v>
+        <v>277</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="O41" s="5" t="s">
-        <v>283</v>
+        <v>41</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>279</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="3">
-        <v>44409.992361111108</v>
-      </c>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
-        <v>71</v>
+        <v>174</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>54</v>
+        <v>169</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2" t="s">
-        <v>109</v>
+        <v>34</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="I42" t="s">
+        <v>176</v>
+      </c>
+      <c r="J42" s="11" t="s">
+        <v>177</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>21</v>
+        <v>315</v>
+      </c>
+      <c r="L42" s="11" t="s">
+        <v>316</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N42" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="O42" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="P42" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="3"/>
-      <c r="B43" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>287</v>
+        <v>33</v>
+      </c>
+      <c r="N42" t="s">
+        <v>179</v>
+      </c>
+      <c r="O42" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="P42" s="13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>249</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="K43" s="2" t="s">
+      <c r="G43" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="L43" s="2" t="s">
-        <v>291</v>
+      <c r="K43" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="L43" s="13" t="s">
+        <v>252</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N43" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="O43" s="2" t="s">
-        <v>293</v>
+        <v>22</v>
+      </c>
+      <c r="N43" t="s">
+        <v>253</v>
+      </c>
+      <c r="O43" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>292</v>
+        <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>105</v>
+      <c r="A44" s="15">
+        <v>44397.036111111112</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>182</v>
+        <v>59</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>176</v>
+        <v>45</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>34</v>
+      <c r="G44" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="I44" t="s">
-        <v>183</v>
+        <v>29</v>
       </c>
       <c r="J44" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>331</v>
+        <v>30</v>
+      </c>
+      <c r="K44" s="11" t="s">
+        <v>312</v>
       </c>
       <c r="L44" s="11" t="s">
-        <v>332</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="M44" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="N44" t="s">
-        <v>186</v>
-      </c>
-      <c r="O44" s="12" t="s">
-        <v>187</v>
+        <v>61</v>
+      </c>
+      <c r="O44" s="14" t="s">
+        <v>62</v>
       </c>
       <c r="P44" s="13" t="s">
-        <v>185</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="15">
+        <v>44411.775694444441</v>
+      </c>
       <c r="B45" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>256</v>
+        <v>76</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>257</v>
+        <v>78</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>241</v>
+        <v>54</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="H45" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H45" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I45" s="11"/>
+      <c r="I45" s="2"/>
       <c r="J45" s="11" t="s">
-        <v>368</v>
+        <v>38</v>
       </c>
       <c r="K45" s="11" t="s">
-        <v>508</v>
+        <v>484</v>
       </c>
       <c r="L45" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
+      </c>
+      <c r="M45" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="N45" t="s">
-        <v>260</v>
-      </c>
-      <c r="O45" s="12" t="s">
-        <v>261</v>
+        <v>80</v>
+      </c>
+      <c r="O45" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="15">
-        <v>44397.036111111112</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>58</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B46" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>59</v>
+        <v>219</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>29</v>
+        <v>258</v>
+      </c>
+      <c r="I46" t="s">
+        <v>176</v>
       </c>
       <c r="J46" s="11" t="s">
-        <v>30</v>
+        <v>325</v>
       </c>
       <c r="K46" s="11" t="s">
-        <v>328</v>
+        <v>230</v>
       </c>
       <c r="L46" s="11" t="s">
-        <v>28</v>
+        <v>221</v>
       </c>
       <c r="M46" s="11" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N46" t="s">
-        <v>61</v>
-      </c>
-      <c r="O46" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="P46" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="15">
-        <v>44411.775694444441</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>76</v>
+        <v>222</v>
+      </c>
+      <c r="O46" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B47" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>77</v>
+        <v>384</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>78</v>
+        <v>385</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>54</v>
+        <v>352</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>79</v>
+        <v>386</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I47" s="2"/>
-      <c r="J47" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K47" s="11" t="s">
-        <v>505</v>
-      </c>
-      <c r="L47" s="13" t="s">
-        <v>28</v>
+        <v>387</v>
+      </c>
+      <c r="J47" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="K47" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="L47" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="M47" s="11" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="N47" t="s">
-        <v>80</v>
-      </c>
-      <c r="O47" s="14" t="s">
-        <v>81</v>
+        <v>389</v>
+      </c>
+      <c r="O47" s="12" t="s">
+        <v>390</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B48" s="2" t="s">
-        <v>225</v>
+        <v>391</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="15">
+        <v>44405.647916666669</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>226</v>
+        <v>92</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>176</v>
+        <v>45</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>227</v>
+        <v>93</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="I48" t="s">
-        <v>183</v>
+        <v>106</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>341</v>
+        <v>94</v>
       </c>
       <c r="K48" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="L48" s="11" t="s">
-        <v>228</v>
+        <v>335</v>
+      </c>
+      <c r="L48" s="13" t="s">
+        <v>336</v>
       </c>
       <c r="M48" s="11" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="N48" t="s">
-        <v>229</v>
+        <v>95</v>
       </c>
       <c r="O48" s="12" t="s">
-        <v>230</v>
+        <v>96</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B49" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>407</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="J49" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="K49" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="L49" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M49" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="N49" t="s">
-        <v>410</v>
-      </c>
-      <c r="O49" s="12" t="s">
-        <v>411</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="15">
-        <v>44405.647916666669</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="J50" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="K50" s="11" t="s">
-        <v>356</v>
-      </c>
-      <c r="L50" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="M50" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="N50" t="s">
-        <v>95</v>
-      </c>
-      <c r="O50" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="P50" s="2" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:P43">
-    <sortCondition ref="C3:C43"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:P41">
+    <sortCondition ref="C3:C41"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="N34" r:id="rId1" xr:uid="{CBF3488F-0731-4784-B778-22BEDC9A87FD}"/>
+    <hyperlink ref="N33" r:id="rId1" xr:uid="{CBF3488F-0731-4784-B778-22BEDC9A87FD}"/>
     <hyperlink ref="O5" r:id="rId2" xr:uid="{AA553A20-924A-4A7A-B3C1-6D6F29D53AB7}"/>
-    <hyperlink ref="O40" r:id="rId3" xr:uid="{9F78E4A3-9753-40AC-9C13-EFA682AF983E}"/>
+    <hyperlink ref="O39" r:id="rId3" xr:uid="{9F78E4A3-9753-40AC-9C13-EFA682AF983E}"/>
     <hyperlink ref="O30" r:id="rId4" xr:uid="{C0B53B11-AD93-46B5-9A27-594CC3A5271C}"/>
     <hyperlink ref="N22" r:id="rId5" xr:uid="{19C35423-B41E-431E-A7D2-61DD10A2F89A}"/>
     <hyperlink ref="O22" r:id="rId6" xr:uid="{FE29F50A-8A83-4CCD-A9E1-9EC92A26530E}"/>
-    <hyperlink ref="O49" r:id="rId7" xr:uid="{365E22B1-13F2-4C32-B64B-BC5B771A124E}"/>
-    <hyperlink ref="O39" r:id="rId8" xr:uid="{EE808F38-5A70-43A7-B847-4DFEFF8C2345}"/>
+    <hyperlink ref="O47" r:id="rId7" xr:uid="{365E22B1-13F2-4C32-B64B-BC5B771A124E}"/>
+    <hyperlink ref="O38" r:id="rId8" xr:uid="{EE808F38-5A70-43A7-B847-4DFEFF8C2345}"/>
     <hyperlink ref="O29" r:id="rId9" xr:uid="{C7957FDB-9E17-4A60-BBEB-6ACA89C74CF0}"/>
     <hyperlink ref="O18" r:id="rId10" xr:uid="{F34024D8-C79C-4E14-91EB-C1D38E6B185F}"/>
     <hyperlink ref="O27" r:id="rId11" xr:uid="{A8E15ABD-7D2B-4B1E-90AD-87A935FE52C9}"/>
     <hyperlink ref="O2" r:id="rId12" xr:uid="{9EFE127E-94E1-4D1A-B4FF-56A0D7F365F6}"/>
     <hyperlink ref="O24" r:id="rId13" xr:uid="{694135F8-96D1-41DA-A6C7-782217CF8081}"/>
     <hyperlink ref="O21" r:id="rId14" xr:uid="{4AFEC0A6-99D6-4CB4-AA7F-2747B52DE82F}"/>
-    <hyperlink ref="O35" r:id="rId15" xr:uid="{1CF56EA4-06F0-461F-9648-39BB0DCA36A3}"/>
+    <hyperlink ref="O34" r:id="rId15" xr:uid="{1CF56EA4-06F0-461F-9648-39BB0DCA36A3}"/>
     <hyperlink ref="N23" r:id="rId16" xr:uid="{59E4A675-78BA-4241-9770-4D060595A68E}"/>
     <hyperlink ref="O23" r:id="rId17" xr:uid="{3A71C51C-0184-4AC7-AFF4-DD100418FA0C}"/>
     <hyperlink ref="N11" r:id="rId18" xr:uid="{DFD50037-4AF8-4266-B9E8-32F987D61850}"/>

</xml_diff>

<commit_message>
Fixed Diana bio and updated How to Join page
</commit_message>
<xml_diff>
--- a/src/data/summerfall23/bios_summerfall23.xlsx
+++ b/src/data/summerfall23/bios_summerfall23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abigailbareiss/dspuci-website-gatsby/src/data/summerfall23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0491F1-A6F7-0945-AF8C-542FFAB2E7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD8C69F-4A97-524D-87B6-B8CFB82965AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="4600" windowWidth="26160" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="860" windowWidth="26160" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -1330,9 +1330,6 @@
     <t>Finance, Strategy, Consulting</t>
   </si>
   <si>
-    <t>Incoming Intern @ FOX Entertainment</t>
-  </si>
-  <si>
     <t>MBA Programs Student Assistant</t>
   </si>
   <si>
@@ -1456,9 +1453,6 @@
     <t>Information Systems, Tech Consulting, Marketing</t>
   </si>
   <si>
-    <t>Data Analytics Inters @ General Atomics - ASI</t>
-  </si>
-  <si>
     <t>Product, Marketing, Strategy</t>
   </si>
   <si>
@@ -1511,6 +1505,12 @@
   </si>
   <si>
     <t>UBA</t>
+  </si>
+  <si>
+    <t>Data Analytics Intern @ General Atomics Aeronautical Systems, Inc.</t>
+  </si>
+  <si>
+    <t>Consumer Insights Intern @ FOX Entertainment</t>
   </si>
 </sst>
 </file>
@@ -1950,10 +1950,10 @@
   <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L22" sqref="L22"/>
+      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2048,13 +2048,13 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="L2" s="16" t="s">
         <v>470</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>471</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>26</v>
@@ -2207,7 +2207,7 @@
         <v>344</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2427,7 +2427,7 @@
         <v>182</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>183</v>
@@ -2447,13 +2447,13 @@
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>458</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>459</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>340</v>
@@ -2462,34 +2462,34 @@
         <v>27</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>37</v>
       </c>
       <c r="I11" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="J11" s="11" t="s">
         <v>461</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="K11" s="11" t="s">
         <v>462</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="L11" s="11" t="s">
         <v>463</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>464</v>
       </c>
       <c r="M11" s="11" t="s">
         <v>26</v>
       </c>
       <c r="N11" s="14" t="s">
+        <v>464</v>
+      </c>
+      <c r="O11" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="O11" s="14" t="s">
+      <c r="P11" s="11" t="s">
         <v>466</v>
-      </c>
-      <c r="P11" s="11" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2522,7 +2522,7 @@
         <v>224</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>225</v>
@@ -2572,7 +2572,7 @@
         <v>163</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>292</v>
@@ -2851,13 +2851,13 @@
         <v>296</v>
       </c>
       <c r="J19" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="L19" s="10" t="s">
         <v>490</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>491</v>
-      </c>
-      <c r="L19" s="10" t="s">
-        <v>492</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>35</v>
@@ -2896,10 +2896,10 @@
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>478</v>
+        <v>495</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>279</v>
@@ -2943,22 +2943,22 @@
         <v>435</v>
       </c>
       <c r="K21" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="L21" s="16" t="s">
         <v>436</v>
-      </c>
-      <c r="L21" s="16" t="s">
-        <v>437</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>41</v>
       </c>
       <c r="N21" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="O21" s="7" t="s">
         <v>438</v>
       </c>
-      <c r="O21" s="7" t="s">
+      <c r="P21" s="2" t="s">
         <v>439</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.15">
@@ -2985,13 +2985,13 @@
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="M22" s="11" t="s">
         <v>25</v>
@@ -3014,7 +3014,7 @@
         <v>114</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>340</v>
@@ -3023,31 +3023,31 @@
         <v>14</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K23" s="11" t="s">
         <v>21</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N23" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="O23" s="12" t="s">
         <v>455</v>
       </c>
-      <c r="O23" s="12" t="s">
-        <v>456</v>
-      </c>
       <c r="P23" s="16" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -3124,13 +3124,13 @@
         <v>40</v>
       </c>
       <c r="J25" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>479</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>481</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>31</v>
@@ -3498,7 +3498,7 @@
         <v>290</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>286</v>
@@ -3519,13 +3519,13 @@
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>340</v>
@@ -3534,32 +3534,32 @@
         <v>14</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="L34" s="16" t="s">
         <v>445</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="L34" s="16" t="s">
-        <v>446</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N34" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="O34" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="O34" s="12" t="s">
+      <c r="P34" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="P34" s="2" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3587,13 +3587,13 @@
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>20</v>
@@ -3640,7 +3640,7 @@
         <v>160</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>50</v>
@@ -3683,10 +3683,10 @@
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>322</v>
@@ -3701,7 +3701,7 @@
         <v>147</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3869,7 +3869,7 @@
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>315</v>
@@ -3887,7 +3887,7 @@
         <v>273</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3964,7 +3964,7 @@
         <v>335</v>
       </c>
       <c r="K43" s="11" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="L43" s="13" t="s">
         <v>248</v>
@@ -4011,7 +4011,7 @@
         <v>30</v>
       </c>
       <c r="K44" s="11" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>28</v>
@@ -4059,7 +4059,7 @@
         <v>38</v>
       </c>
       <c r="K45" s="11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="L45" s="13" t="s">
         <v>28</v>
@@ -4153,7 +4153,7 @@
         <v>374</v>
       </c>
       <c r="L47" s="11" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="M47" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Changed names of files from quarter names to current_data so they don't need to be manually changed in future quarters.
</commit_message>
<xml_diff>
--- a/src/data/summerfall23/bios_summerfall23.xlsx
+++ b/src/data/summerfall23/bios_summerfall23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abigailbareiss/dspuci-website-gatsby/src/data/summerfall23/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicalin/dsp_vs_code/dspuci-website-gatsby/src/data/summerfall23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F199C54-5FD4-EE42-B6F2-79AFFDA6AE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEEC777-CB2E-D647-AA69-8D388219D6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="860" windowWidth="26160" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="740" windowWidth="26160" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -1048,9 +1048,6 @@
     <t>San Ramon, CA</t>
   </si>
   <si>
-    <t>Hiking Club at UCI</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/abigailbareiss/</t>
   </si>
   <si>
@@ -1511,6 +1508,9 @@
   </si>
   <si>
     <t>Consumer Insights Intern @ FOX Entertainment</t>
+  </si>
+  <si>
+    <t>Product, Hiking Club at UCI</t>
   </si>
 </sst>
 </file>
@@ -1950,10 +1950,10 @@
   <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2026,13 +2026,13 @@
     <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>417</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>340</v>
@@ -2041,32 +2041,32 @@
         <v>18</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="L2" s="16" t="s">
         <v>469</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>470</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>419</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2195,19 +2195,19 @@
         <v>21</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>342</v>
+        <v>496</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="N5" t="s">
+        <v>342</v>
+      </c>
+      <c r="O5" s="12" t="s">
         <v>343</v>
       </c>
-      <c r="O5" s="12" t="s">
-        <v>344</v>
-      </c>
       <c r="P5" s="16" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2427,7 +2427,7 @@
         <v>182</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>183</v>
@@ -2447,13 +2447,13 @@
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>457</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>458</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>340</v>
@@ -2462,34 +2462,34 @@
         <v>27</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>37</v>
       </c>
       <c r="I11" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="J11" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="K11" s="11" t="s">
         <v>461</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="L11" s="11" t="s">
         <v>462</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>463</v>
       </c>
       <c r="M11" s="11" t="s">
         <v>26</v>
       </c>
       <c r="N11" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="O11" s="14" t="s">
         <v>464</v>
       </c>
-      <c r="O11" s="14" t="s">
+      <c r="P11" s="11" t="s">
         <v>465</v>
-      </c>
-      <c r="P11" s="11" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2522,7 +2522,7 @@
         <v>224</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>225</v>
@@ -2572,7 +2572,7 @@
         <v>163</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>292</v>
@@ -2662,7 +2662,7 @@
         <v>314</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>21</v>
@@ -2782,13 +2782,13 @@
     <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>400</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>340</v>
@@ -2804,25 +2804,25 @@
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>33</v>
       </c>
       <c r="N18" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="O18" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="O18" s="7" t="s">
+      <c r="P18" s="16" t="s">
         <v>404</v>
-      </c>
-      <c r="P18" s="16" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="14" x14ac:dyDescent="0.15">
@@ -2851,13 +2851,13 @@
         <v>296</v>
       </c>
       <c r="J19" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="K19" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="K19" s="9" t="s">
+      <c r="L19" s="10" t="s">
         <v>489</v>
-      </c>
-      <c r="L19" s="10" t="s">
-        <v>490</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>35</v>
@@ -2896,10 +2896,10 @@
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>279</v>
@@ -2919,13 +2919,13 @@
     </row>
     <row r="21" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>433</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>434</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>340</v>
@@ -2934,42 +2934,42 @@
         <v>27</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J21" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="L21" s="16" t="s">
         <v>435</v>
-      </c>
-      <c r="K21" s="16" t="s">
-        <v>496</v>
-      </c>
-      <c r="L21" s="16" t="s">
-        <v>436</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>41</v>
       </c>
       <c r="N21" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="O21" s="7" t="s">
         <v>437</v>
       </c>
-      <c r="O21" s="7" t="s">
+      <c r="P21" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.15">
       <c r="B22" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>114</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>340</v>
@@ -2978,32 +2978,32 @@
         <v>27</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>118</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="16" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="M22" s="11" t="s">
         <v>25</v>
       </c>
       <c r="N22" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="O22" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="O22" s="7" t="s">
+      <c r="P22" s="16" t="s">
         <v>368</v>
-      </c>
-      <c r="P22" s="16" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3014,7 +3014,7 @@
         <v>114</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>340</v>
@@ -3023,42 +3023,42 @@
         <v>14</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K23" s="11" t="s">
         <v>21</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N23" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="O23" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="O23" s="12" t="s">
-        <v>455</v>
-      </c>
       <c r="P23" s="16" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B24" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>114</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>340</v>
@@ -3073,13 +3073,13 @@
         <v>118</v>
       </c>
       <c r="I24" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="J24" s="16" t="s">
         <v>426</v>
       </c>
-      <c r="J24" s="16" t="s">
+      <c r="K24" s="16" t="s">
         <v>427</v>
-      </c>
-      <c r="K24" s="16" t="s">
-        <v>428</v>
       </c>
       <c r="L24" s="16" t="s">
         <v>286</v>
@@ -3088,13 +3088,13 @@
         <v>33</v>
       </c>
       <c r="N24" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="O24" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="O24" s="7" t="s">
+      <c r="P24" s="16" t="s">
         <v>430</v>
-      </c>
-      <c r="P24" s="16" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -3124,13 +3124,13 @@
         <v>40</v>
       </c>
       <c r="J25" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="L25" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>479</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>31</v>
@@ -3165,7 +3165,7 @@
         <v>195</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I26" t="s">
         <v>197</v>
@@ -3194,13 +3194,13 @@
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>340</v>
@@ -3209,31 +3209,31 @@
         <v>14</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="H27" s="16" t="s">
         <v>408</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>409</v>
       </c>
       <c r="J27" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K27" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="L27" s="16" t="s">
         <v>410</v>
-      </c>
-      <c r="L27" s="16" t="s">
-        <v>411</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N27" t="s">
+        <v>411</v>
+      </c>
+      <c r="O27" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="O27" s="7" t="s">
+      <c r="P27" s="2" t="s">
         <v>413</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3285,13 +3285,13 @@
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>390</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>340</v>
@@ -3303,40 +3303,40 @@
         <v>117</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I29" s="16"/>
       <c r="J29" s="16" t="s">
+        <v>391</v>
+      </c>
+      <c r="K29" s="16" t="s">
         <v>392</v>
       </c>
-      <c r="K29" s="16" t="s">
-        <v>393</v>
-      </c>
       <c r="L29" s="16" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M29" s="16" t="s">
         <v>31</v>
       </c>
       <c r="N29" t="s">
+        <v>393</v>
+      </c>
+      <c r="O29" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="O29" s="7" t="s">
-        <v>395</v>
-      </c>
       <c r="P29" s="16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>357</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>340</v>
@@ -3354,25 +3354,25 @@
         <v>107</v>
       </c>
       <c r="J30" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="L30" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>360</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N30" t="s">
+        <v>360</v>
+      </c>
+      <c r="O30" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="O30" s="7" t="s">
+      <c r="P30" s="16" t="s">
         <v>362</v>
-      </c>
-      <c r="P30" s="16" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3395,7 +3395,7 @@
         <v>262</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>327</v>
@@ -3498,7 +3498,7 @@
         <v>290</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>286</v>
@@ -3519,13 +3519,13 @@
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>441</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>442</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>340</v>
@@ -3534,32 +3534,32 @@
         <v>14</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="L34" s="16" t="s">
         <v>444</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="L34" s="16" t="s">
-        <v>445</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N34" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="O34" s="12" t="s">
         <v>446</v>
       </c>
-      <c r="O34" s="12" t="s">
+      <c r="P34" s="2" t="s">
         <v>447</v>
-      </c>
-      <c r="P34" s="2" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3587,13 +3587,13 @@
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>20</v>
@@ -3640,7 +3640,7 @@
         <v>160</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>50</v>
@@ -3683,10 +3683,10 @@
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>322</v>
@@ -3701,19 +3701,19 @@
         <v>147</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>380</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>340</v>
@@ -3722,44 +3722,44 @@
         <v>14</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="K38" s="16" t="s">
         <v>382</v>
       </c>
-      <c r="K38" s="16" t="s">
+      <c r="L38" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>384</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="O38" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="P38" s="16" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>347</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>340</v>
@@ -3768,32 +3768,32 @@
         <v>27</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="K39" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="K39" s="16" t="s">
+      <c r="L39" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>351</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>35</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O39" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3869,7 +3869,7 @@
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>315</v>
@@ -3887,7 +3887,7 @@
         <v>273</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3964,7 +3964,7 @@
         <v>335</v>
       </c>
       <c r="K43" s="11" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L43" s="13" t="s">
         <v>248</v>
@@ -4011,7 +4011,7 @@
         <v>30</v>
       </c>
       <c r="K44" s="11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>28</v>
@@ -4059,7 +4059,7 @@
         <v>38</v>
       </c>
       <c r="K45" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="L45" s="13" t="s">
         <v>28</v>
@@ -4126,13 +4126,13 @@
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>371</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>372</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>340</v>
@@ -4141,7 +4141,7 @@
         <v>14</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H47" s="11" t="s">
         <v>106</v>
@@ -4150,22 +4150,22 @@
         <v>108</v>
       </c>
       <c r="K47" s="16" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="L47" s="11" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="M47" s="11" t="s">
         <v>26</v>
       </c>
       <c r="N47" t="s">
+        <v>374</v>
+      </c>
+      <c r="O47" s="12" t="s">
         <v>375</v>
       </c>
-      <c r="O47" s="12" t="s">
+      <c r="P47" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="P47" s="2" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>